<commit_message>
forcasting error band fix
</commit_message>
<xml_diff>
--- a/examples/test_q.xlsx
+++ b/examples/test_q.xlsx
@@ -331,7 +331,7 @@
     <t>SBFVAR</t>
   </si>
   <si>
-    <t>2025-04-16 11:26</t>
+    <t>2025-04-30 14:52</t>
   </si>
   <si>
     <t>Q</t>
@@ -2497,22 +2497,22 @@
         <v>84</v>
       </c>
       <c r="B79">
-        <v>-0.02750878568375196</v>
+        <v>0.0589423938925807</v>
       </c>
       <c r="C79">
-        <v>0.006758952094373832</v>
+        <v>0.009166667368066274</v>
       </c>
       <c r="D79">
-        <v>-0.009232957876897815</v>
+        <v>-0.0217679952112962</v>
       </c>
       <c r="E79">
-        <v>-0.03483995019100791</v>
+        <v>0.06313165332251804</v>
       </c>
       <c r="F79">
-        <v>-0.0146709832189497</v>
+        <v>-0.04963330386911739</v>
       </c>
       <c r="G79">
-        <v>-0.09113472865747187</v>
+        <v>-0.01824944274686772</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -2520,22 +2520,22 @@
         <v>85</v>
       </c>
       <c r="B80">
-        <v>0.06133096819485845</v>
+        <v>0.004907273770271612</v>
       </c>
       <c r="C80">
-        <v>0.007183203387366897</v>
+        <v>-0.003216443796962212</v>
       </c>
       <c r="D80">
-        <v>0.01519523826513737</v>
+        <v>0.02563122437606987</v>
       </c>
       <c r="E80">
-        <v>0.07771165140401126</v>
+        <v>-0.002874176503164186</v>
       </c>
       <c r="F80">
-        <v>-0.02051114910772991</v>
+        <v>0.01186897232683281</v>
       </c>
       <c r="G80">
-        <v>0.3055393511458283</v>
+        <v>-0.1298984141248347</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -2543,22 +2543,22 @@
         <v>86</v>
       </c>
       <c r="B81">
-        <v>0.07924606401067369</v>
+        <v>-0.02364601523043436</v>
       </c>
       <c r="C81">
-        <v>0.018285502822617</v>
+        <v>-0.003464008412092047</v>
       </c>
       <c r="D81">
-        <v>0.04898729396112699</v>
+        <v>0.03216322516619648</v>
       </c>
       <c r="E81">
-        <v>0.05857746148910647</v>
+        <v>-0.01355943487238542</v>
       </c>
       <c r="F81">
-        <v>0.02281511984248742</v>
+        <v>0.02085492681530928</v>
       </c>
       <c r="G81">
-        <v>0.1838257508739881</v>
+        <v>0.169616362240307</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -2566,22 +2566,22 @@
         <v>87</v>
       </c>
       <c r="B82">
-        <v>0.01782122770780332</v>
+        <v>0.0401107485453099</v>
       </c>
       <c r="C82">
-        <v>0.02793355501443251</v>
+        <v>0.0168355899532709</v>
       </c>
       <c r="D82">
-        <v>0.01984920267049625</v>
+        <v>0.0663201152322281</v>
       </c>
       <c r="E82">
-        <v>0.07709167036524547</v>
+        <v>0.06368474351608769</v>
       </c>
       <c r="F82">
-        <v>-0.008144007663142088</v>
+        <v>0.01231257339162343</v>
       </c>
       <c r="G82">
-        <v>0.2298898230465761</v>
+        <v>-0.174400219243848</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -2589,22 +2589,22 @@
         <v>88</v>
       </c>
       <c r="B83">
-        <v>0.02734142948445869</v>
+        <v>0.009539413916455977</v>
       </c>
       <c r="C83">
-        <v>0.0123924531512142</v>
+        <v>-9.386561326377163E-05</v>
       </c>
       <c r="D83">
-        <v>-0.006538302336238764</v>
+        <v>0.05295569624791095</v>
       </c>
       <c r="E83">
-        <v>0.0391748349344715</v>
+        <v>0.0007916218481727868</v>
       </c>
       <c r="F83">
-        <v>-0.01129135451588611</v>
+        <v>0.04558913123680412</v>
       </c>
       <c r="G83">
-        <v>0.07890425132244851</v>
+        <v>0.004103506866313866</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -2612,22 +2612,22 @@
         <v>89</v>
       </c>
       <c r="B84">
-        <v>0.02618365202900143</v>
+        <v>-0.007505161418278765</v>
       </c>
       <c r="C84">
-        <v>-0.04279708103009849</v>
+        <v>0.00457937536948687</v>
       </c>
       <c r="D84">
-        <v>-0.004201290093139605</v>
+        <v>0.04766680125980742</v>
       </c>
       <c r="E84">
-        <v>0.03272449721305715</v>
+        <v>0.02767964478570226</v>
       </c>
       <c r="F84">
-        <v>-0.0406691320127355</v>
+        <v>-0.01276421443936309</v>
       </c>
       <c r="G84">
-        <v>0.1757849711026954</v>
+        <v>-0.0434129228494578</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -2635,22 +2635,22 @@
         <v>90</v>
       </c>
       <c r="B85">
-        <v>0.02071161772244713</v>
+        <v>0.03792242499881065</v>
       </c>
       <c r="C85">
-        <v>0.01014144851263175</v>
+        <v>0.03422513979404068</v>
       </c>
       <c r="D85">
-        <v>0.01305632928996401</v>
+        <v>0.08412715640269375</v>
       </c>
       <c r="E85">
-        <v>0.02212159452789939</v>
+        <v>-4.440138462490639E-05</v>
       </c>
       <c r="F85">
-        <v>-0.0005508895664943427</v>
+        <v>0.00837933233059689</v>
       </c>
       <c r="G85">
-        <v>-0.08300770372720764</v>
+        <v>-0.01613260226056533</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -2658,22 +2658,22 @@
         <v>91</v>
       </c>
       <c r="B86">
-        <v>-0.02065205901326796</v>
+        <v>-0.004576567590228327</v>
       </c>
       <c r="C86">
-        <v>0.009056489503049008</v>
+        <v>-0.02228823581795109</v>
       </c>
       <c r="D86">
-        <v>0.06548228125235427</v>
+        <v>0.0072020460993309</v>
       </c>
       <c r="E86">
-        <v>-0.03568253592602016</v>
+        <v>-0.01146533469400185</v>
       </c>
       <c r="F86">
-        <v>0.05708771460881175</v>
+        <v>0.03684821772384615</v>
       </c>
       <c r="G86">
-        <v>0.2402839650096412</v>
+        <v>0.0810513605837796</v>
       </c>
     </row>
   </sheetData>
@@ -4488,22 +4488,22 @@
         <v>84</v>
       </c>
       <c r="B79">
-        <v>-0.05876308386920223</v>
+        <v>0.06287225612920666</v>
       </c>
       <c r="C79">
-        <v>0.004540184497857362</v>
+        <v>0.01555847309831074</v>
       </c>
       <c r="D79">
-        <v>0.01196592651887363</v>
+        <v>-0.01963809495119482</v>
       </c>
       <c r="E79">
-        <v>-0.04661730600567371</v>
+        <v>0.05608865200817329</v>
       </c>
       <c r="F79">
-        <v>-0.03103329965108529</v>
+        <v>-0.06969862289944562</v>
       </c>
       <c r="G79">
-        <v>-0.07034309447066261</v>
+        <v>-0.01964882903761871</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -4511,22 +4511,22 @@
         <v>85</v>
       </c>
       <c r="B80">
-        <v>0.04180972318872675</v>
+        <v>0.02015146190765047</v>
       </c>
       <c r="C80">
-        <v>-0.009244482846657581</v>
+        <v>-0.02272803453739647</v>
       </c>
       <c r="D80">
-        <v>0.02264518230876215</v>
+        <v>0.006970315334761834</v>
       </c>
       <c r="E80">
-        <v>0.09466254591412705</v>
+        <v>0.03418272344008388</v>
       </c>
       <c r="F80">
-        <v>-0.05919749781862559</v>
+        <v>0.0166910434715713</v>
       </c>
       <c r="G80">
-        <v>0.239682529813851</v>
+        <v>-0.18300956433661</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -4534,22 +4534,22 @@
         <v>86</v>
       </c>
       <c r="B81">
-        <v>0.04054301957105151</v>
+        <v>-0.04138853960868276</v>
       </c>
       <c r="C81">
-        <v>0.02225600268598062</v>
+        <v>-0.01451596651567854</v>
       </c>
       <c r="D81">
-        <v>0.05258684079718708</v>
+        <v>0.03795124466923137</v>
       </c>
       <c r="E81">
-        <v>0.0755400212774601</v>
+        <v>-0.02903823505704206</v>
       </c>
       <c r="F81">
-        <v>0.02636401943136575</v>
+        <v>0.04531438203842102</v>
       </c>
       <c r="G81">
-        <v>0.3016492515169465</v>
+        <v>0.1510776659928775</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -4557,22 +4557,22 @@
         <v>87</v>
       </c>
       <c r="B82">
-        <v>0.01903913568824524</v>
+        <v>0.03319987106344347</v>
       </c>
       <c r="C82">
-        <v>0.04454334276732274</v>
+        <v>0.03562858575426645</v>
       </c>
       <c r="D82">
-        <v>0.002911984545270595</v>
+        <v>0.0277770137678798</v>
       </c>
       <c r="E82">
-        <v>0.09851908383151337</v>
+        <v>0.07363744169585612</v>
       </c>
       <c r="F82">
-        <v>0.00426035540917662</v>
+        <v>0.03444709552843701</v>
       </c>
       <c r="G82">
-        <v>0.231651754706579</v>
+        <v>-0.1775122733166334</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -4580,22 +4580,22 @@
         <v>88</v>
       </c>
       <c r="B83">
-        <v>0.02118035269575839</v>
+        <v>-0.01222179724561359</v>
       </c>
       <c r="C83">
-        <v>0.001860844259898529</v>
+        <v>0.003660958429620543</v>
       </c>
       <c r="D83">
-        <v>-0.01719684289804494</v>
+        <v>0.03156142469202472</v>
       </c>
       <c r="E83">
-        <v>0.03254464220952644</v>
+        <v>0.009028878845272145</v>
       </c>
       <c r="F83">
-        <v>-0.006325054951557868</v>
+        <v>0.01822485911411993</v>
       </c>
       <c r="G83">
-        <v>0.1200797023443685</v>
+        <v>-0.2144736409748667</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -4603,22 +4603,22 @@
         <v>89</v>
       </c>
       <c r="B84">
-        <v>0.02694589182044578</v>
+        <v>-0.04182531437007755</v>
       </c>
       <c r="C84">
-        <v>-0.04879800838309998</v>
+        <v>-0.0008485132581453087</v>
       </c>
       <c r="D84">
-        <v>0.009959742960817043</v>
+        <v>0.03948247906779799</v>
       </c>
       <c r="E84">
-        <v>0.03469497630870765</v>
+        <v>0.005751967620175241</v>
       </c>
       <c r="F84">
-        <v>-0.05684491449762062</v>
+        <v>-0.03881425272338383</v>
       </c>
       <c r="G84">
-        <v>0.2119147214242704</v>
+        <v>-0.1635380071433752</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -4626,22 +4626,22 @@
         <v>90</v>
       </c>
       <c r="B85">
-        <v>-0.02063176796550533</v>
+        <v>0.08281718992618181</v>
       </c>
       <c r="C85">
-        <v>0.006876102754664324</v>
+        <v>0.03475001610065352</v>
       </c>
       <c r="D85">
-        <v>-0.01306481292825771</v>
+        <v>0.0782412080233621</v>
       </c>
       <c r="E85">
-        <v>0.006000637556764566</v>
+        <v>-0.01020509774849661</v>
       </c>
       <c r="F85">
-        <v>-0.001433318237073685</v>
+        <v>0.01072328732333653</v>
       </c>
       <c r="G85">
-        <v>-0.03996598854572087</v>
+        <v>0.04808540812739278</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -4649,22 +4649,22 @@
         <v>91</v>
       </c>
       <c r="B86">
-        <v>-0.0249222637565313</v>
+        <v>0.03788043927351746</v>
       </c>
       <c r="C86">
-        <v>0.01039702750589057</v>
+        <v>-0.03251139097231533</v>
       </c>
       <c r="D86">
-        <v>0.06553056436423314</v>
+        <v>0.007759538674444488</v>
       </c>
       <c r="E86">
-        <v>-0.04113330638850182</v>
+        <v>-0.0286810660744025</v>
       </c>
       <c r="F86">
-        <v>0.004911248251824776</v>
+        <v>0.06146362444673873</v>
       </c>
       <c r="G86">
-        <v>0.1558579346661217</v>
+        <v>0.1817654536200237</v>
       </c>
     </row>
   </sheetData>
@@ -5555,22 +5555,22 @@
         <v>84</v>
       </c>
       <c r="B79">
-        <v>0.09398729458487341</v>
+        <v>0.1283322461890762</v>
       </c>
       <c r="C79">
-        <v>0.06218872120202242</v>
+        <v>0.07317976017410575</v>
       </c>
       <c r="D79">
-        <v>0.04213265089295817</v>
+        <v>0.08354754411926593</v>
       </c>
       <c r="E79">
-        <v>0.1002614396328446</v>
+        <v>0.1937099849978076</v>
       </c>
       <c r="F79">
-        <v>0.147327793085308</v>
+        <v>0.06096316011908902</v>
       </c>
       <c r="G79">
-        <v>0.4966287252565897</v>
+        <v>0.6777909129742926</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -5578,22 +5578,22 @@
         <v>85</v>
       </c>
       <c r="B80">
-        <v>0.244589630215835</v>
+        <v>0.1399589671639684</v>
       </c>
       <c r="C80">
-        <v>0.1178532619990855</v>
+        <v>0.09223256322915047</v>
       </c>
       <c r="D80">
-        <v>0.14267176276697</v>
+        <v>0.1577362471959261</v>
       </c>
       <c r="E80">
-        <v>0.2426425450193489</v>
+        <v>0.189684496277074</v>
       </c>
       <c r="F80">
-        <v>0.2106314721393837</v>
+        <v>0.1142519829914635</v>
       </c>
       <c r="G80">
-        <v>1.082895459397533</v>
+        <v>0.5966991458717956</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -5601,22 +5601,22 @@
         <v>86</v>
       </c>
       <c r="B81">
-        <v>0.2665742151490024</v>
+        <v>0.1766366478432785</v>
       </c>
       <c r="C81">
-        <v>0.0745092355398934</v>
+        <v>0.09211865681739073</v>
       </c>
       <c r="D81">
-        <v>0.155261402271608</v>
+        <v>0.1242220279177425</v>
       </c>
       <c r="E81">
-        <v>0.2110818245613429</v>
+        <v>0.1996022748996165</v>
       </c>
       <c r="F81">
-        <v>0.2038122357855273</v>
+        <v>0.1229589239604931</v>
       </c>
       <c r="G81">
-        <v>0.5861884842476699</v>
+        <v>0.9798371865604463</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -5624,22 +5624,22 @@
         <v>87</v>
       </c>
       <c r="B82">
-        <v>0.1514111274891199</v>
+        <v>0.191965554455431</v>
       </c>
       <c r="C82">
-        <v>0.08681557799905003</v>
+        <v>0.08610833423076444</v>
       </c>
       <c r="D82">
-        <v>0.1186756959311896</v>
+        <v>0.2073699571861236</v>
       </c>
       <c r="E82">
-        <v>0.1600779304519259</v>
+        <v>0.1649429254891797</v>
       </c>
       <c r="F82">
-        <v>0.07493087145695196</v>
+        <v>0.1165971283701741</v>
       </c>
       <c r="G82">
-        <v>0.8042762196653603</v>
+        <v>0.6717619645737785</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -5647,22 +5647,22 @@
         <v>88</v>
       </c>
       <c r="B83">
-        <v>0.218854946111218</v>
+        <v>0.215701945491799</v>
       </c>
       <c r="C83">
-        <v>0.09276278135424793</v>
+        <v>0.0805157893713055</v>
       </c>
       <c r="D83">
-        <v>0.1163835938541682</v>
+        <v>0.226911215224349</v>
       </c>
       <c r="E83">
-        <v>0.2378491200142487</v>
+        <v>0.1043454777736658</v>
       </c>
       <c r="F83">
-        <v>0.09478903350752914</v>
+        <v>0.2414747846652874</v>
       </c>
       <c r="G83">
-        <v>0.6213670291859306</v>
+        <v>1.027004432394623</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -5670,22 +5670,22 @@
         <v>89</v>
       </c>
       <c r="B84">
-        <v>0.1874146904674953</v>
+        <v>0.1519424979025993</v>
       </c>
       <c r="C84">
-        <v>0.02798785520760113</v>
+        <v>0.05029838503403285</v>
       </c>
       <c r="D84">
-        <v>0.07396116319392144</v>
+        <v>0.193511838560721</v>
       </c>
       <c r="E84">
-        <v>0.1093272188977071</v>
+        <v>0.2562692463647355</v>
       </c>
       <c r="F84">
-        <v>0.0918554141944268</v>
+        <v>0.1531277047648166</v>
       </c>
       <c r="G84">
-        <v>0.709053588677008</v>
+        <v>0.8038587180466954</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -5693,22 +5693,22 @@
         <v>90</v>
       </c>
       <c r="B85">
-        <v>0.2409742892223019</v>
+        <v>0.1723750678763493</v>
       </c>
       <c r="C85">
-        <v>0.06452783619403613</v>
+        <v>0.1136887164172046</v>
       </c>
       <c r="D85">
-        <v>0.155811267439571</v>
+        <v>0.1832304699800382</v>
       </c>
       <c r="E85">
-        <v>0.1781316657237502</v>
+        <v>0.132858785564291</v>
       </c>
       <c r="F85">
-        <v>0.1567224594671414</v>
+        <v>0.05968863086563728</v>
       </c>
       <c r="G85">
-        <v>0.4831095028602788</v>
+        <v>0.7199625048796281</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -5716,22 +5716,22 @@
         <v>91</v>
       </c>
       <c r="B86">
-        <v>0.09262003908916584</v>
+        <v>0.1702438085807875</v>
       </c>
       <c r="C86">
-        <v>0.08865965018769643</v>
+        <v>0.03666847852070018</v>
       </c>
       <c r="D86">
-        <v>0.1764029863841278</v>
+        <v>0.1339316895864138</v>
       </c>
       <c r="E86">
-        <v>0.10111360021578</v>
+        <v>0.08147911169195288</v>
       </c>
       <c r="F86">
-        <v>0.3007140206099963</v>
+        <v>0.1347823963512346</v>
       </c>
       <c r="G86">
-        <v>0.8851588379359272</v>
+        <v>0.7006887699053593</v>
       </c>
     </row>
   </sheetData>
@@ -6622,22 +6622,22 @@
         <v>84</v>
       </c>
       <c r="B79">
-        <v>-0.1227687700502138</v>
+        <v>-0.03530454397075036</v>
       </c>
       <c r="C79">
-        <v>-0.0564404148707119</v>
+        <v>-0.08152088903548685</v>
       </c>
       <c r="D79">
-        <v>-0.0868803997636638</v>
+        <v>-0.1237431566336094</v>
       </c>
       <c r="E79">
-        <v>-0.168539819953084</v>
+        <v>-0.07016735983044567</v>
       </c>
       <c r="F79">
-        <v>-0.1268537574162849</v>
+        <v>-0.1377223244069615</v>
       </c>
       <c r="G79">
-        <v>-0.5810962034803104</v>
+        <v>-0.5070045054249239</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -6645,22 +6645,22 @@
         <v>85</v>
       </c>
       <c r="B80">
-        <v>-0.05329190450806138</v>
+        <v>-0.1784301829217816</v>
       </c>
       <c r="C80">
-        <v>-0.06903190750784099</v>
+        <v>-0.06310000528685647</v>
       </c>
       <c r="D80">
-        <v>-0.1375892593039713</v>
+        <v>-0.09229757338176409</v>
       </c>
       <c r="E80">
-        <v>-0.08619937444748094</v>
+        <v>-0.2024518288433304</v>
       </c>
       <c r="F80">
-        <v>-0.2006761289704523</v>
+        <v>-0.0986670615198286</v>
       </c>
       <c r="G80">
-        <v>-0.4617351758546335</v>
+        <v>-0.6362250066179113</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -6668,22 +6668,22 @@
         <v>86</v>
       </c>
       <c r="B81">
-        <v>-0.08763154685786417</v>
+        <v>-0.2217990620568021</v>
       </c>
       <c r="C81">
-        <v>-0.05363811272820461</v>
+        <v>-0.07797186295829237</v>
       </c>
       <c r="D81">
-        <v>-0.07515330251686113</v>
+        <v>-0.06952379032777273</v>
       </c>
       <c r="E81">
-        <v>-0.1201609950783669</v>
+        <v>-0.2055467307488613</v>
       </c>
       <c r="F81">
-        <v>-0.2071777433997091</v>
+        <v>-0.1307954122599474</v>
       </c>
       <c r="G81">
-        <v>-0.4035109923175031</v>
+        <v>-0.5280570185289749</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -6691,22 +6691,22 @@
         <v>87</v>
       </c>
       <c r="B82">
-        <v>-0.0777745762995852</v>
+        <v>-0.05139399363618324</v>
       </c>
       <c r="C82">
-        <v>-0.05459682581919432</v>
+        <v>-0.04471975233534934</v>
       </c>
       <c r="D82">
-        <v>-0.0567203960484944</v>
+        <v>-0.01158553429938786</v>
       </c>
       <c r="E82">
-        <v>-0.04866651502124898</v>
+        <v>-0.03482550005738858</v>
       </c>
       <c r="F82">
-        <v>-0.1183583577730931</v>
+        <v>-0.09935263098878609</v>
       </c>
       <c r="G82">
-        <v>-0.2563406544265583</v>
+        <v>-1.062032773393138</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -6714,22 +6714,22 @@
         <v>88</v>
       </c>
       <c r="B83">
-        <v>-0.09959704207607639</v>
+        <v>-0.1164260042546646</v>
       </c>
       <c r="C83">
-        <v>-0.03683487835800914</v>
+        <v>-0.1058290094454175</v>
       </c>
       <c r="D83">
-        <v>-0.1012125059810492</v>
+        <v>-0.04384988215472466</v>
       </c>
       <c r="E83">
-        <v>-0.1296650490183324</v>
+        <v>-0.1207835675089434</v>
       </c>
       <c r="F83">
-        <v>-0.1188400563575504</v>
+        <v>-0.09566438733965221</v>
       </c>
       <c r="G83">
-        <v>-0.5322757492295322</v>
+        <v>-0.6126268941433971</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -6737,22 +6737,22 @@
         <v>89</v>
       </c>
       <c r="B84">
-        <v>-0.1032831439079342</v>
+        <v>-0.1411560808747468</v>
       </c>
       <c r="C84">
-        <v>-0.1037980491976603</v>
+        <v>-0.02550916883352519</v>
       </c>
       <c r="D84">
-        <v>-0.1010678014414043</v>
+        <v>-0.05621373427229301</v>
       </c>
       <c r="E84">
-        <v>-0.04516455485738737</v>
+        <v>-0.1266913208130431</v>
       </c>
       <c r="F84">
-        <v>-0.1391293938248012</v>
+        <v>-0.1278827130044926</v>
       </c>
       <c r="G84">
-        <v>-0.4979717686964444</v>
+        <v>-0.8107722466624163</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -6760,22 +6760,22 @@
         <v>90</v>
       </c>
       <c r="B85">
-        <v>-0.121090854572914</v>
+        <v>-0.1881347008222534</v>
       </c>
       <c r="C85">
-        <v>-0.04375833600502658</v>
+        <v>-0.05085393103713844</v>
       </c>
       <c r="D85">
-        <v>-0.08160737412729385</v>
+        <v>-0.001606301741261838</v>
       </c>
       <c r="E85">
-        <v>-0.1212382077120855</v>
+        <v>-0.1115162910151004</v>
       </c>
       <c r="F85">
-        <v>-0.1288551915082928</v>
+        <v>-0.06330443901973465</v>
       </c>
       <c r="G85">
-        <v>-0.5951268030353134</v>
+        <v>-0.8218147726624092</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -6783,22 +6783,22 @@
         <v>91</v>
       </c>
       <c r="B86">
-        <v>-0.1283541743249408</v>
+        <v>-0.2079542306924398</v>
       </c>
       <c r="C86">
-        <v>-0.06904501302482342</v>
+        <v>-0.07770591177479427</v>
       </c>
       <c r="D86">
-        <v>-0.04290492128764848</v>
+        <v>-0.1405035985559561</v>
       </c>
       <c r="E86">
-        <v>-0.1620090761507979</v>
+        <v>-0.0814206968429855</v>
       </c>
       <c r="F86">
-        <v>-0.1174667625446741</v>
+        <v>-0.1218026208178659</v>
       </c>
       <c r="G86">
-        <v>-0.2092363090969579</v>
+        <v>-0.6533414427428841</v>
       </c>
     </row>
   </sheetData>
@@ -7689,22 +7689,22 @@
         <v>84</v>
       </c>
       <c r="B79">
-        <v>0.07433518260338756</v>
+        <v>0.1048697892533126</v>
       </c>
       <c r="C79">
-        <v>0.05100643749956396</v>
+        <v>0.06448918939078685</v>
       </c>
       <c r="D79">
-        <v>0.02036918870317769</v>
+        <v>0.04470848573911724</v>
       </c>
       <c r="E79">
-        <v>0.06072150485110198</v>
+        <v>0.1505306362380864</v>
       </c>
       <c r="F79">
-        <v>0.0753213690588844</v>
+        <v>0.02642305077724779</v>
       </c>
       <c r="G79">
-        <v>0.2902779974901132</v>
+        <v>0.2675073763352058</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -7712,22 +7712,22 @@
         <v>85</v>
       </c>
       <c r="B80">
-        <v>0.132189568992627</v>
+        <v>0.1040691511592851</v>
       </c>
       <c r="C80">
-        <v>0.05551367563595579</v>
+        <v>0.04053793907872476</v>
       </c>
       <c r="D80">
-        <v>0.1099778271962535</v>
+        <v>0.1295240574501012</v>
       </c>
       <c r="E80">
-        <v>0.1698925404199226</v>
+        <v>0.08046344613267602</v>
       </c>
       <c r="F80">
-        <v>0.1649614767558091</v>
+        <v>0.09360322417166705</v>
       </c>
       <c r="G80">
-        <v>0.8394467075107955</v>
+        <v>0.2497824254621088</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -7735,22 +7735,22 @@
         <v>86</v>
       </c>
       <c r="B81">
-        <v>0.2320253513129592</v>
+        <v>0.1155287364943511</v>
       </c>
       <c r="C81">
-        <v>0.05447909298303284</v>
+        <v>0.02971854287714027</v>
       </c>
       <c r="D81">
-        <v>0.133836872902478</v>
+        <v>0.09752241583307213</v>
       </c>
       <c r="E81">
-        <v>0.1683220517581537</v>
+        <v>0.1458780426395408</v>
       </c>
       <c r="F81">
-        <v>0.1785433154393668</v>
+        <v>0.1113268733408183</v>
       </c>
       <c r="G81">
-        <v>0.511517407384477</v>
+        <v>0.5468929134204096</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -7758,22 +7758,22 @@
         <v>87</v>
       </c>
       <c r="B82">
-        <v>0.08502555320031308</v>
+        <v>0.09449293915982054</v>
       </c>
       <c r="C82">
-        <v>0.08103394307181469</v>
+        <v>0.06882965740227985</v>
       </c>
       <c r="D82">
-        <v>0.0725794138640337</v>
+        <v>0.1409231924163393</v>
       </c>
       <c r="E82">
-        <v>0.1502539918294322</v>
+        <v>0.1064551940567053</v>
       </c>
       <c r="F82">
-        <v>0.03877966208949764</v>
+        <v>0.105055918752924</v>
       </c>
       <c r="G82">
-        <v>0.4265867274193044</v>
+        <v>0.24085068130308</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -7781,22 +7781,22 @@
         <v>88</v>
       </c>
       <c r="B83">
-        <v>0.06439037663957303</v>
+        <v>0.1301741129091992</v>
       </c>
       <c r="C83">
-        <v>0.04714175547202593</v>
+        <v>0.07330706560105377</v>
       </c>
       <c r="D83">
-        <v>0.05833826418317118</v>
+        <v>0.1529577643519031</v>
       </c>
       <c r="E83">
-        <v>0.1956250959184317</v>
+        <v>0.08696881582160206</v>
       </c>
       <c r="F83">
-        <v>0.0655745258157935</v>
+        <v>0.1824949271751023</v>
       </c>
       <c r="G83">
-        <v>0.3396677222048491</v>
+        <v>0.6297855414370195</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -7804,22 +7804,22 @@
         <v>89</v>
       </c>
       <c r="B84">
-        <v>0.1077374509511493</v>
+        <v>0.137887763852923</v>
       </c>
       <c r="C84">
-        <v>0.01121320654476046</v>
+        <v>0.04056835322747501</v>
       </c>
       <c r="D84">
-        <v>0.05534952654493276</v>
+        <v>0.119135246031652</v>
       </c>
       <c r="E84">
-        <v>0.09200651874042183</v>
+        <v>0.1269821917271561</v>
       </c>
       <c r="F84">
-        <v>0.04025310142171104</v>
+        <v>0.07820424726721822</v>
       </c>
       <c r="G84">
-        <v>0.5343992343327751</v>
+        <v>0.6596264099721788</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -7827,22 +7827,22 @@
         <v>90</v>
       </c>
       <c r="B85">
-        <v>0.1041014991741565</v>
+        <v>0.1200970436453171</v>
       </c>
       <c r="C85">
-        <v>0.05309064613670497</v>
+        <v>0.09609304104491266</v>
       </c>
       <c r="D85">
-        <v>0.1113793783038559</v>
+        <v>0.134128994891981</v>
       </c>
       <c r="E85">
-        <v>0.1186236360586586</v>
+        <v>0.03988913484549034</v>
       </c>
       <c r="F85">
-        <v>0.08542848983707735</v>
+        <v>0.05280021045067589</v>
       </c>
       <c r="G85">
-        <v>0.1192504497212763</v>
+        <v>0.5469012756807425</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -7850,22 +7850,22 @@
         <v>91</v>
       </c>
       <c r="B86">
-        <v>0.0627566776120988</v>
+        <v>0.1456045680085854</v>
       </c>
       <c r="C86">
-        <v>0.05391933004576935</v>
+        <v>0.02144932367810945</v>
       </c>
       <c r="D86">
-        <v>0.1496331878255329</v>
+        <v>0.08588320361290998</v>
       </c>
       <c r="E86">
-        <v>0.06322126610304205</v>
+        <v>0.03966357998259145</v>
       </c>
       <c r="F86">
-        <v>0.2491054659802138</v>
+        <v>0.09383834574320064</v>
       </c>
       <c r="G86">
-        <v>0.7343037032437145</v>
+        <v>0.4064742599891062</v>
       </c>
     </row>
   </sheetData>
@@ -8756,22 +8756,22 @@
         <v>84</v>
       </c>
       <c r="B79">
-        <v>-0.112167912736494</v>
+        <v>0.00146122449683319</v>
       </c>
       <c r="C79">
-        <v>-0.02458557284725232</v>
+        <v>-0.04398601436680132</v>
       </c>
       <c r="D79">
-        <v>-0.06084666536384743</v>
+        <v>-0.09334448611847308</v>
       </c>
       <c r="E79">
-        <v>-0.1259852938431283</v>
+        <v>-0.01072175917852745</v>
       </c>
       <c r="F79">
-        <v>-0.1097802145620585</v>
+        <v>-0.1001068541762262</v>
       </c>
       <c r="G79">
-        <v>-0.5600918517307323</v>
+        <v>-0.4451487388092242</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -8779,22 +8779,22 @@
         <v>85</v>
       </c>
       <c r="B80">
-        <v>-0.01568552045048989</v>
+        <v>-0.08260351029447999</v>
       </c>
       <c r="C80">
-        <v>-0.04675484601941836</v>
+        <v>-0.04881001583292129</v>
       </c>
       <c r="D80">
-        <v>-0.08189698109473613</v>
+        <v>-0.0707032793864843</v>
       </c>
       <c r="E80">
-        <v>-0.03888111814108758</v>
+        <v>-0.1978882201891558</v>
       </c>
       <c r="F80">
-        <v>-0.1782590498771215</v>
+        <v>-0.07590396387504338</v>
       </c>
       <c r="G80">
-        <v>-0.1216152817713023</v>
+        <v>-0.6317281095576071</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -8802,22 +8802,22 @@
         <v>86</v>
       </c>
       <c r="B81">
-        <v>-0.03179487676202924</v>
+        <v>-0.1347174139407966</v>
       </c>
       <c r="C81">
-        <v>-0.009815815693410838</v>
+        <v>-0.05045718226329066</v>
       </c>
       <c r="D81">
-        <v>-0.03107472039798532</v>
+        <v>-0.0477047058215617</v>
       </c>
       <c r="E81">
-        <v>-0.04580946047472988</v>
+        <v>-0.1426584438745372</v>
       </c>
       <c r="F81">
-        <v>-0.1109969922346739</v>
+        <v>-0.08365634177556498</v>
       </c>
       <c r="G81">
-        <v>-0.2010268662563196</v>
+        <v>-0.3743022004703418</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -8825,22 +8825,22 @@
         <v>87</v>
       </c>
       <c r="B82">
-        <v>-0.07116346826136032</v>
+        <v>-0.04785210615146233</v>
       </c>
       <c r="C82">
-        <v>-0.02900541672924831</v>
+        <v>-0.0429127809077799</v>
       </c>
       <c r="D82">
-        <v>-0.04170166044782055</v>
+        <v>-0.0008665670399138495</v>
       </c>
       <c r="E82">
-        <v>-0.01498002355511387</v>
+        <v>-0.01065472172990461</v>
       </c>
       <c r="F82">
-        <v>-0.07610428881184936</v>
+        <v>-0.09039072104424964</v>
       </c>
       <c r="G82">
-        <v>-0.03392428678105593</v>
+        <v>-0.7331693537166446</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -8848,22 +8848,22 @@
         <v>88</v>
       </c>
       <c r="B83">
-        <v>-0.07120443083319673</v>
+        <v>-0.07187010574359408</v>
       </c>
       <c r="C83">
-        <v>-0.02504628724340046</v>
+        <v>-0.08292750537678063</v>
       </c>
       <c r="D83">
-        <v>-0.08743991254200045</v>
+        <v>-0.03468861795430871</v>
       </c>
       <c r="E83">
-        <v>-0.1076896980404293</v>
+        <v>-0.07614567236804115</v>
       </c>
       <c r="F83">
-        <v>-0.1009791898009727</v>
+        <v>-0.03775973830426442</v>
       </c>
       <c r="G83">
-        <v>-0.1876324453217808</v>
+        <v>-0.5140433984601233</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -8871,22 +8871,22 @@
         <v>89</v>
       </c>
       <c r="B84">
-        <v>-0.04834844745783505</v>
+        <v>-0.1199196198988565</v>
       </c>
       <c r="C84">
-        <v>-0.09158064536271046</v>
+        <v>-0.02402185152083603</v>
       </c>
       <c r="D84">
-        <v>-0.05675558971788814</v>
+        <v>-0.03649402204485042</v>
       </c>
       <c r="E84">
-        <v>-0.03696983150930468</v>
+        <v>-0.1002186344050213</v>
       </c>
       <c r="F84">
-        <v>-0.1215431155103015</v>
+        <v>-0.1053642278098185</v>
       </c>
       <c r="G84">
-        <v>-0.1122915756187298</v>
+        <v>-0.5368616385010038</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -8894,22 +8894,22 @@
         <v>90</v>
       </c>
       <c r="B85">
-        <v>-0.0868299504939104</v>
+        <v>-0.05216329891098969</v>
       </c>
       <c r="C85">
-        <v>-0.02935306275034869</v>
+        <v>-0.03614036492645638</v>
       </c>
       <c r="D85">
-        <v>-0.07084389075922534</v>
+        <v>0.03401673179810549</v>
       </c>
       <c r="E85">
-        <v>-0.07886857353365492</v>
+        <v>-0.0610836779554268</v>
       </c>
       <c r="F85">
-        <v>-0.08192442962342809</v>
+        <v>-0.01743400259426854</v>
       </c>
       <c r="G85">
-        <v>-0.390393320465561</v>
+        <v>-0.3989970755392562</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -8917,22 +8917,22 @@
         <v>91</v>
       </c>
       <c r="B86">
-        <v>-0.0910054171262458</v>
+        <v>-0.1794031008595345</v>
       </c>
       <c r="C86">
-        <v>-0.04312897266101549</v>
+        <v>-0.05307894831363566</v>
       </c>
       <c r="D86">
-        <v>-0.02388291785349928</v>
+        <v>-0.05490211567782976</v>
       </c>
       <c r="E86">
-        <v>-0.1349769748417202</v>
+        <v>-0.06932282588726268</v>
       </c>
       <c r="F86">
-        <v>-0.07620224407918073</v>
+        <v>-0.02003103986504034</v>
       </c>
       <c r="G86">
-        <v>-0.1770259817842044</v>
+        <v>-0.4295315656427894</v>
       </c>
     </row>
   </sheetData>

</xml_diff>